<commit_message>
updated new leagues on birthday
</commit_message>
<xml_diff>
--- a/Divisions/G1.xlsx
+++ b/Divisions/G1.xlsx
@@ -17,13 +17,12 @@
     <sheet name="Red Totals" r:id="rId11" sheetId="9"/>
     <sheet name="OVUN" r:id="rId12" sheetId="10"/>
     <sheet name="Shots Analysis" r:id="rId13" sheetId="11"/>
-    <sheet name="L6" r:id="rId14" sheetId="12"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3904" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3785" uniqueCount="368">
   <si>
     <t>Team</t>
   </si>
@@ -1127,321 +1126,6 @@
   </si>
   <si>
     <t>25.81%</t>
-  </si>
-  <si>
-    <t>Form</t>
-  </si>
-  <si>
-    <t>Goals scored</t>
-  </si>
-  <si>
-    <t>Goals conceded</t>
-  </si>
-  <si>
-    <t>Total Goals</t>
-  </si>
-  <si>
-    <t>CSForm</t>
-  </si>
-  <si>
-    <t>Win Margin</t>
-  </si>
-  <si>
-    <t>Team against</t>
-  </si>
-  <si>
-    <t>AEK,W D D W L L</t>
-  </si>
-  <si>
-    <t>Apollon,L W W D L D</t>
-  </si>
-  <si>
-    <t>Aris,D D W L W D</t>
-  </si>
-  <si>
-    <t>Asteras Tripolis,W L L W D W</t>
-  </si>
-  <si>
-    <t>Atromitos,L W D D L L</t>
-  </si>
-  <si>
-    <t>Giannina,D L D W D L</t>
-  </si>
-  <si>
-    <t>Ionikos,D L W L L W</t>
-  </si>
-  <si>
-    <t>Lamia,W L W W W D</t>
-  </si>
-  <si>
-    <t>OFI Crete,W L L W D W</t>
-  </si>
-  <si>
-    <t>Olympiakos,W D D W L L</t>
-  </si>
-  <si>
-    <t>Panathinaikos,L W W W W W</t>
-  </si>
-  <si>
-    <t>Panetolikos,D D D D W L</t>
-  </si>
-  <si>
-    <t>PAOK,W D L L L W</t>
-  </si>
-  <si>
-    <t>Volos NFC,L W L D L D</t>
-  </si>
-  <si>
-    <t>AEK,3 1 0 3 2 2,(11)</t>
-  </si>
-  <si>
-    <t>Apollon,0 1 2 1 1 0,(5)</t>
-  </si>
-  <si>
-    <t>Aris,0 0 1 0 3 2,(6)</t>
-  </si>
-  <si>
-    <t>Asteras Tripolis,2 0 0 1 2 3,(8)</t>
-  </si>
-  <si>
-    <t>Atromitos,1 2 0 1 0 0,(4)</t>
-  </si>
-  <si>
-    <t>Giannina,0 2 1 1 0 0,(4)</t>
-  </si>
-  <si>
-    <t>Ionikos,0 2 5 0 0 3,(10)</t>
-  </si>
-  <si>
-    <t>Lamia,3 1 3 1 1 0,(9)</t>
-  </si>
-  <si>
-    <t>OFI Crete,2 0 0 2 0 1,(5)</t>
-  </si>
-  <si>
-    <t>Olympiakos,2 1 1 3 1 0,(8)</t>
-  </si>
-  <si>
-    <t>Panathinaikos,0 1 2 1 4 3,(11)</t>
-  </si>
-  <si>
-    <t>Panetolikos,0 0 0 0 2 0,(2)</t>
-  </si>
-  <si>
-    <t>PAOK,1 1 1 0 1 2,(6)</t>
-  </si>
-  <si>
-    <t>Volos NFC,1 3 0 1 0 1,(6)</t>
-  </si>
-  <si>
-    <t>AEK,2 1 0 0 3 3,(9)</t>
-  </si>
-  <si>
-    <t>Apollon,1 0 1 1 5 0,(8)</t>
-  </si>
-  <si>
-    <t>Aris,0 0 0 1 2 2,(5)</t>
-  </si>
-  <si>
-    <t>Asteras Tripolis,1 1 2 0 2 0,(6)</t>
-  </si>
-  <si>
-    <t>Atromitos,2 0 0 1 1 1,(5)</t>
-  </si>
-  <si>
-    <t>Giannina,0 3 1 0 0 3,(7)</t>
-  </si>
-  <si>
-    <t>Ionikos,0 3 1 3 4 1,(12)</t>
-  </si>
-  <si>
-    <t>Lamia,2 2 2 0 0 0,(6)</t>
-  </si>
-  <si>
-    <t>OFI Crete,1 3 1 0 0 0,(5)</t>
-  </si>
-  <si>
-    <t>Olympiakos,1 1 1 2 2 5,(12)</t>
-  </si>
-  <si>
-    <t>Panathinaikos,1 0 1 0 0 2,(4)</t>
-  </si>
-  <si>
-    <t>Panetolikos,0 0 0 0 1 2,(3)</t>
-  </si>
-  <si>
-    <t>PAOK,0 1 2 1 3 0,(7)</t>
-  </si>
-  <si>
-    <t>Volos NFC,2 0 1 1 1 1,(6)</t>
-  </si>
-  <si>
-    <t>AEK,5 2 0 3 5 5,(20)</t>
-  </si>
-  <si>
-    <t>Apollon,1 1 3 2 6 0,(13)</t>
-  </si>
-  <si>
-    <t>Aris,0 0 1 1 5 4,(11)</t>
-  </si>
-  <si>
-    <t>Asteras Tripolis,3 1 2 1 4 3,(14)</t>
-  </si>
-  <si>
-    <t>Atromitos,3 2 0 2 1 1,(9)</t>
-  </si>
-  <si>
-    <t>Giannina,0 5 2 1 0 3,(11)</t>
-  </si>
-  <si>
-    <t>Ionikos,0 5 6 3 4 4,(22)</t>
-  </si>
-  <si>
-    <t>Lamia,5 3 5 1 1 0,(15)</t>
-  </si>
-  <si>
-    <t>OFI Crete,3 3 1 2 0 1,(10)</t>
-  </si>
-  <si>
-    <t>Olympiakos,3 2 2 5 3 5,(20)</t>
-  </si>
-  <si>
-    <t>Panathinaikos,1 1 3 1 4 5,(15)</t>
-  </si>
-  <si>
-    <t>Panetolikos,0 0 0 0 3 2,(5)</t>
-  </si>
-  <si>
-    <t>PAOK,1 2 3 1 4 2,(13)</t>
-  </si>
-  <si>
-    <t>Volos NFC,3 3 1 2 1 2,(12)</t>
-  </si>
-  <si>
-    <t>AEK,2-3 1-1 0-0 3-0 3-2 2-3</t>
-  </si>
-  <si>
-    <t>Apollon,1-0 1-0 1-2 1-1 5-1 0-0</t>
-  </si>
-  <si>
-    <t>Aris,0-0 0-0 1-0 0-1 3-2 2-2</t>
-  </si>
-  <si>
-    <t>Asteras Tripolis,1-2 1-0 0-2 0-1 2-2 0-3</t>
-  </si>
-  <si>
-    <t>Atromitos,2-1 0-2 0-0 1-1 0-1 1-0</t>
-  </si>
-  <si>
-    <t>Giannina,0-0 2-3 1-1 1-0 0-0 0-3</t>
-  </si>
-  <si>
-    <t>Ionikos,0-0 3-2 5-1 3-0 4-0 3-1</t>
-  </si>
-  <si>
-    <t>Lamia,2-3 1-2 2-3 0-1 0-1 0-0</t>
-  </si>
-  <si>
-    <t>OFI Crete,1-2 3-0 0-1 0-2 0-0 1-0</t>
-  </si>
-  <si>
-    <t>Olympiakos,1-2 1-1 1-1 3-2 1-2 5-0</t>
-  </si>
-  <si>
-    <t>Panathinaikos,1-0 1-0 1-2 0-1 4-0 2-3</t>
-  </si>
-  <si>
-    <t>Panetolikos,0-0 0-0 0-0 0-0 1-2 2-0</t>
-  </si>
-  <si>
-    <t>PAOK,0-1 1-1 1-2 0-1 3-1 2-0</t>
-  </si>
-  <si>
-    <t>Volos NFC,2-1 3-0 1-0 1-1 1-0 1-1</t>
-  </si>
-  <si>
-    <t>AEK,1 0 0 3 -1 -1,(2)</t>
-  </si>
-  <si>
-    <t>Apollon,-1 1 1 0 -4 0,(-3)</t>
-  </si>
-  <si>
-    <t>Aris,0 0 1 -1 1 0,(1)</t>
-  </si>
-  <si>
-    <t>Asteras Tripolis,1 -1 -2 1 0 3,(2)</t>
-  </si>
-  <si>
-    <t>Atromitos,-1 2 0 0 -1 -1,(-1)</t>
-  </si>
-  <si>
-    <t>Giannina,0 -1 0 1 0 -3,(-3)</t>
-  </si>
-  <si>
-    <t>Ionikos,0 -1 4 -3 -4 2,(-2)</t>
-  </si>
-  <si>
-    <t>Lamia,1 -1 1 1 1 0,(3)</t>
-  </si>
-  <si>
-    <t>OFI Crete,1 -3 -1 2 0 1,(0)</t>
-  </si>
-  <si>
-    <t>Olympiakos,1 0 0 1 -1 -5,(-4)</t>
-  </si>
-  <si>
-    <t>Panathinaikos,-1 1 1 1 4 1,(7)</t>
-  </si>
-  <si>
-    <t>Panetolikos,0 0 0 0 1 -2,(-1)</t>
-  </si>
-  <si>
-    <t>PAOK,1 0 -1 -1 -2 2,(-1)</t>
-  </si>
-  <si>
-    <t>Volos NFC,-1 3 -1 0 -1 0,(0)</t>
-  </si>
-  <si>
-    <t>AEK,Giannina(6) PAOK(2) Panathinaikos(4) Giannina(6) Aris(3) Olympiakos(1)</t>
-  </si>
-  <si>
-    <t>Apollon,Atromitos(12) Panetolikos(11) OFI Crete(8) Volos NFC(10) Ionikos(7) Lamia(13)</t>
-  </si>
-  <si>
-    <t>Aris,Panathinaikos(4) Giannina(6) PAOK(2) Olympiakos(1) AEK(5) Asteras Tripolis(9)</t>
-  </si>
-  <si>
-    <t>Asteras Tripolis,AEK(5) Panathinaikos(4) Lamia(13) PAOK(2) Apollon Apollon() Giannina(6)</t>
-  </si>
-  <si>
-    <t>Atromitos,AEK(5) Volos NFC(10) Panetolikos(11) OFI Crete(8) Ionikos(7) OFI Crete(8)</t>
-  </si>
-  <si>
-    <t>Giannina,Panathinaikos(4) AEK(5) Volos NFC(10) PAOK(2) Lamia(13) Aris(3)</t>
-  </si>
-  <si>
-    <t>Ionikos,Aris(3) Olympiakos(1) Apollon(14) AEK(5) Panathinaikos(4) Panetolikos(11)</t>
-  </si>
-  <si>
-    <t>Lamia,OFI Crete(8) OFI Crete(8) Asteras Tripolis(9) Lamia(13) Atromitos(12) Atromitos(12)</t>
-  </si>
-  <si>
-    <t>OFI Crete,Panetolikos(11) Volos NFC(10) Panetolikos(11) Asteras Tripolis(9) Apollon(14) Asteras Tripolis(9)</t>
-  </si>
-  <si>
-    <t>Olympiakos,Lamia(13) AEK(5) Atromitos(12) Giannina(6) Panathinaikos(4) Volos NFC(10)</t>
-  </si>
-  <si>
-    <t>Panathinaikos,Panathinaikos(4) Aris(3) PAOK(2) Aris(3) Giannina(6) AEK(5)</t>
-  </si>
-  <si>
-    <t>Panetolikos,Giannina(6) Asteras Tripolis(9) Volos NFC(10) AEK(5) Olympiakos(1) PAOK(2)</t>
-  </si>
-  <si>
-    <t>PAOK,OFI Crete(8) AEK(5) Olympiakos(1) Aris(3) Ionikos(7) Panathinaikos(4)</t>
-  </si>
-  <si>
-    <t>Volos NFC,Panathinaikos(4) Lamia(13) Aris(3) Atromitos(12) Giannina(6) Olympiakos(1)</t>
   </si>
 </sst>
 </file>
@@ -3857,407 +3541,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1"/>
-      <c r="B1" t="s">
-        <v>368</v>
-      </c>
-      <c r="C1" t="s">
-        <v>369</v>
-      </c>
-      <c r="D1" t="s">
-        <v>370</v>
-      </c>
-      <c r="E1" t="s">
-        <v>371</v>
-      </c>
-      <c r="F1" t="s">
-        <v>372</v>
-      </c>
-      <c r="G1" t="s">
-        <v>373</v>
-      </c>
-      <c r="H1" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>375</v>
-      </c>
-      <c r="C2" t="s">
-        <v>389</v>
-      </c>
-      <c r="D2" t="s">
-        <v>403</v>
-      </c>
-      <c r="E2" t="s">
-        <v>417</v>
-      </c>
-      <c r="F2" t="s">
-        <v>431</v>
-      </c>
-      <c r="G2" t="s">
-        <v>445</v>
-      </c>
-      <c r="H2" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>376</v>
-      </c>
-      <c r="C3" t="s">
-        <v>390</v>
-      </c>
-      <c r="D3" t="s">
-        <v>404</v>
-      </c>
-      <c r="E3" t="s">
-        <v>418</v>
-      </c>
-      <c r="F3" t="s">
-        <v>432</v>
-      </c>
-      <c r="G3" t="s">
-        <v>446</v>
-      </c>
-      <c r="H3" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>377</v>
-      </c>
-      <c r="C4" t="s">
-        <v>391</v>
-      </c>
-      <c r="D4" t="s">
-        <v>405</v>
-      </c>
-      <c r="E4" t="s">
-        <v>419</v>
-      </c>
-      <c r="F4" t="s">
-        <v>433</v>
-      </c>
-      <c r="G4" t="s">
-        <v>447</v>
-      </c>
-      <c r="H4" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>378</v>
-      </c>
-      <c r="C5" t="s">
-        <v>392</v>
-      </c>
-      <c r="D5" t="s">
-        <v>406</v>
-      </c>
-      <c r="E5" t="s">
-        <v>420</v>
-      </c>
-      <c r="F5" t="s">
-        <v>434</v>
-      </c>
-      <c r="G5" t="s">
-        <v>448</v>
-      </c>
-      <c r="H5" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>379</v>
-      </c>
-      <c r="C6" t="s">
-        <v>393</v>
-      </c>
-      <c r="D6" t="s">
-        <v>407</v>
-      </c>
-      <c r="E6" t="s">
-        <v>421</v>
-      </c>
-      <c r="F6" t="s">
-        <v>435</v>
-      </c>
-      <c r="G6" t="s">
-        <v>449</v>
-      </c>
-      <c r="H6" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>380</v>
-      </c>
-      <c r="C7" t="s">
-        <v>394</v>
-      </c>
-      <c r="D7" t="s">
-        <v>408</v>
-      </c>
-      <c r="E7" t="s">
-        <v>422</v>
-      </c>
-      <c r="F7" t="s">
-        <v>436</v>
-      </c>
-      <c r="G7" t="s">
-        <v>450</v>
-      </c>
-      <c r="H7" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>381</v>
-      </c>
-      <c r="C8" t="s">
-        <v>395</v>
-      </c>
-      <c r="D8" t="s">
-        <v>409</v>
-      </c>
-      <c r="E8" t="s">
-        <v>423</v>
-      </c>
-      <c r="F8" t="s">
-        <v>437</v>
-      </c>
-      <c r="G8" t="s">
-        <v>451</v>
-      </c>
-      <c r="H8" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>382</v>
-      </c>
-      <c r="C9" t="s">
-        <v>396</v>
-      </c>
-      <c r="D9" t="s">
-        <v>410</v>
-      </c>
-      <c r="E9" t="s">
-        <v>424</v>
-      </c>
-      <c r="F9" t="s">
-        <v>438</v>
-      </c>
-      <c r="G9" t="s">
-        <v>452</v>
-      </c>
-      <c r="H9" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>383</v>
-      </c>
-      <c r="C10" t="s">
-        <v>397</v>
-      </c>
-      <c r="D10" t="s">
-        <v>411</v>
-      </c>
-      <c r="E10" t="s">
-        <v>425</v>
-      </c>
-      <c r="F10" t="s">
-        <v>439</v>
-      </c>
-      <c r="G10" t="s">
-        <v>453</v>
-      </c>
-      <c r="H10" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" t="s">
-        <v>384</v>
-      </c>
-      <c r="C11" t="s">
-        <v>398</v>
-      </c>
-      <c r="D11" t="s">
-        <v>412</v>
-      </c>
-      <c r="E11" t="s">
-        <v>426</v>
-      </c>
-      <c r="F11" t="s">
-        <v>440</v>
-      </c>
-      <c r="G11" t="s">
-        <v>454</v>
-      </c>
-      <c r="H11" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" t="s">
-        <v>385</v>
-      </c>
-      <c r="C12" t="s">
-        <v>399</v>
-      </c>
-      <c r="D12" t="s">
-        <v>413</v>
-      </c>
-      <c r="E12" t="s">
-        <v>427</v>
-      </c>
-      <c r="F12" t="s">
-        <v>441</v>
-      </c>
-      <c r="G12" t="s">
-        <v>455</v>
-      </c>
-      <c r="H12" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" t="s">
-        <v>386</v>
-      </c>
-      <c r="C13" t="s">
-        <v>400</v>
-      </c>
-      <c r="D13" t="s">
-        <v>414</v>
-      </c>
-      <c r="E13" t="s">
-        <v>428</v>
-      </c>
-      <c r="F13" t="s">
-        <v>442</v>
-      </c>
-      <c r="G13" t="s">
-        <v>456</v>
-      </c>
-      <c r="H13" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" t="s">
-        <v>387</v>
-      </c>
-      <c r="C14" t="s">
-        <v>401</v>
-      </c>
-      <c r="D14" t="s">
-        <v>415</v>
-      </c>
-      <c r="E14" t="s">
-        <v>429</v>
-      </c>
-      <c r="F14" t="s">
-        <v>443</v>
-      </c>
-      <c r="G14" t="s">
-        <v>457</v>
-      </c>
-      <c r="H14" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" t="s">
-        <v>388</v>
-      </c>
-      <c r="C15" t="s">
-        <v>402</v>
-      </c>
-      <c r="D15" t="s">
-        <v>416</v>
-      </c>
-      <c r="E15" t="s">
-        <v>430</v>
-      </c>
-      <c r="F15" t="s">
-        <v>444</v>
-      </c>
-      <c r="G15" t="s">
-        <v>458</v>
-      </c>
-      <c r="H15" t="s">
-        <v>472</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>

</xml_diff>